<commit_message>
Fix: Implemented Log In, Log out & Data extraction
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\FastPipe_Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13FA2C2-38C1-4FBD-AF4D-47212F98905B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA190170-8731-4FD7-A3A6-1B065A9EA1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="16980" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -165,7 +165,10 @@
     <t>Site_Link</t>
   </si>
   <si>
-    <t>https://app.panteratools.com</t>
+    <t>Pantera_Credentials</t>
+  </si>
+  <si>
+    <t>https://app.panteratools.com/#signin</t>
   </si>
 </sst>
 </file>
@@ -553,7 +556,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -637,10 +640,17 @@
         <v>45</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
         <v>46</v>
       </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1633,7 +1643,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{D6A2B05B-FC45-47FC-9726-7A94A02B102C}"/>
+    <hyperlink ref="B8" r:id="rId1" location="signin" xr:uid="{D6A2B05B-FC45-47FC-9726-7A94A02B102C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Fix: Improved the queueing logic
- Implemented duplicate validation
- Introduced Transaction Status Excel to track transactions
- Relocated the Extract Pantera Bids workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\FastPipe_Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA190170-8731-4FD7-A3A6-1B065A9EA1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDEEC51-95A5-407A-AEE6-DFF34441466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="16980" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1654,7 +1654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Feat: Implemented file extraction
- Implemented file extraction
- Implmented folder renaming and moving to destination folder
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\FastPipe_Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDEEC51-95A5-407A-AEE6-DFF34441466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4768E2-34E8-4BC4-828B-F58102D087EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>https://app.panteratools.com/#signin</t>
+  </si>
+  <si>
+    <t>Download_Folder_Path</t>
+  </si>
+  <si>
+    <t>C:\Users\FredrickMutua\Documents\Bids Folder</t>
+  </si>
+  <si>
+    <t>Bids_Destination_Folder_Path</t>
+  </si>
+  <si>
+    <t>C:\Users\FredrickMutua\Documents\UiPath Test Folder</t>
   </si>
 </sst>
 </file>
@@ -555,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -652,8 +664,22 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Minor Prod changes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\FastPipe_Automation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\UiPath\Fast_Pipe_Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4768E2-34E8-4BC4-828B-F58102D087EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BCFE2D-D46B-4904-9C72-52EE838D7472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -174,13 +174,13 @@
     <t>Download_Folder_Path</t>
   </si>
   <si>
-    <t>C:\Users\FredrickMutua\Documents\Bids Folder</t>
-  </si>
-  <si>
     <t>Bids_Destination_Folder_Path</t>
   </si>
   <si>
-    <t>C:\Users\FredrickMutua\Documents\UiPath Test Folder</t>
+    <t>C:\Users\CatherineNyaguthiiMw\Downloads\Bids Download</t>
+  </si>
+  <si>
+    <t>C:\Users\CatherineNyaguthiiMw\Dahlonega Group\Bids_Drawings - Documents\United Plumbing\FastEST-Local.site\Jobs</t>
   </si>
 </sst>
 </file>
@@ -568,15 +568,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -624,7 +624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -634,7 +634,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -669,12 +669,12 @@
         <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>51</v>
@@ -1680,16 +1680,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1726,7 +1726,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1851,7 +1851,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2845,12 +2845,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Fix: Implemented FastPipe upload
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\UiPath\Fast_Pipe_Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BCFE2D-D46B-4904-9C72-52EE838D7472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1E7530-B692-4744-8CFA-FA7BFFCD2977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Feat: Release of V1.0.5
- Introduced a new report template format
- Improved all error handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\UiPath\Fast_Pipe_Automation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\FastPipe_Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1E7530-B692-4744-8CFA-FA7BFFCD2977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42585F11-BE0E-45AD-87B1-80D476721409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -567,16 +567,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -624,7 +624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -634,7 +634,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1680,16 +1680,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1726,7 +1726,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1851,7 +1851,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2845,12 +2845,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>